<commit_message>
more logs + status enum check on DTO
</commit_message>
<xml_diff>
--- a/backend/error_example.xlsx
+++ b/backend/error_example.xlsx
@@ -52,7 +52,7 @@
     <t>2024-06-15</t>
   </si>
   <si>
-    <t>asdf</t>
+    <t>Jakiś Pan</t>
   </si>
   <si>
     <t>zrealizowana</t>
@@ -95,11 +95,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -371,7 +374,10 @@
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2">
+        <v>12348.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="1" t="s">

</xml_diff>